<commit_message>
Update harp camp timetable by replacing the existing timetable file and removing outdated student timetable files for multiple participants to streamline resources.
</commit_message>
<xml_diff>
--- a/input/harp-campA-time-table.xlsx
+++ b/input/harp-campA-time-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Python\summer-camp-time-table\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5EAF39-992D-444C-85AF-E0CEC5379B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01676B29-4668-4B68-9472-664336B97E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6720" yWindow="1425" windowWidth="22050" windowHeight="13425" activeTab="4" xr2:uid="{E318233D-D99F-47E3-BC58-6A555949ADA4}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="53">
   <si>
     <t>Sivan MEGAN</t>
   </si>
@@ -193,12 +193,6 @@
     <t>Teacher</t>
   </si>
   <si>
-    <t>H2, H3, H4, H5, H6, H9 Observe MasterClass by Liya HUANG (Room Liya)</t>
-  </si>
-  <si>
-    <t>H1, H3, H5, H6, H7, H8 Observe MasterClass by Sivan MEGAN (Room Sivan)</t>
-  </si>
-  <si>
     <t>Harp MasterClass by Liya HUANG
 H1, H7, H8 
 (Room Liya)</t>
@@ -215,6 +209,18 @@
     <t>Harp MasterClass by Gwyneth WENTINK
 H3, H5, H6
 (Room GW)</t>
+  </si>
+  <si>
+    <t>H2, H3, H4, H5, H6, H9, H10, H11, H12 Observe MasterClass by Liya HUANG (Room Liya)</t>
+  </si>
+  <si>
+    <t>H3, H5, H6, H10, H11, H12 Observe MasterClass by Liya HUANG (Room Liya)</t>
+  </si>
+  <si>
+    <t>H1, H3, H5, H6, H7, H8,H10, H11, H12 Observe MasterClass by Sivan MEGAN (Room Sivan)</t>
+  </si>
+  <si>
+    <t>H1, H7, H8,H10, H11, H12 Observe MasterClass by Sivan MEGAN (Room Sivan)</t>
   </si>
 </sst>
 </file>
@@ -293,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -491,17 +497,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -522,9 +517,49 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -536,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -555,14 +590,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -599,16 +646,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -617,94 +658,73 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -725,6 +745,71 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1106,89 +1191,89 @@
       <c r="A3" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1238,31 +1323,31 @@
       <c r="A11" s="5">
         <v>0.5</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1312,103 +1397,103 @@
       <c r="A15" s="5">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="13" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1458,27 +1543,27 @@
       <c r="A24" s="5">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -1487,7 +1572,7 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="14"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -1501,7 +1586,7 @@
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -1515,7 +1600,7 @@
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
@@ -1526,34 +1611,34 @@
       <c r="A28" s="5">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="14"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="14"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -1564,10 +1649,10 @@
       <c r="A30" s="5">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="14"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="14"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
@@ -1578,10 +1663,10 @@
       <c r="A31" s="5">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
@@ -1606,13 +1691,13 @@
       <c r="A33" s="5">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E33" s="4"/>
@@ -1719,40 +1804,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="D33:D39"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="C33:C39"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="C28:C31"/>
     <mergeCell ref="J24:J27"/>
     <mergeCell ref="H24:H27"/>
     <mergeCell ref="I24:I27"/>
@@ -1769,6 +1820,40 @@
     <mergeCell ref="I11:I14"/>
     <mergeCell ref="B20:B23"/>
     <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D33:D39"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="B33:B39"/>
+    <mergeCell ref="C33:C39"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1822,87 +1907,87 @@
       <c r="A3" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1952,29 +2037,29 @@
       <c r="A11" s="5">
         <v>0.5</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10" t="s">
+      <c r="I11" s="13"/>
+      <c r="J11" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2024,101 +2109,101 @@
       <c r="A15" s="5">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10" t="s">
+      <c r="F20" s="13"/>
+      <c r="G20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2168,27 +2253,27 @@
       <c r="A24" s="5">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -2197,7 +2282,7 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="14"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -2211,7 +2296,7 @@
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -2225,7 +2310,7 @@
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
@@ -2236,34 +2321,34 @@
       <c r="A28" s="5">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="14"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="14"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -2274,10 +2359,10 @@
       <c r="A30" s="5">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="14"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="14"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
@@ -2288,10 +2373,10 @@
       <c r="A31" s="5">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
@@ -2316,13 +2401,13 @@
       <c r="A33" s="5">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E33" s="4"/>
@@ -2423,44 +2508,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="B3:J6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="J7:J10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="J11:J14"/>
-    <mergeCell ref="B15:J19"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
     <mergeCell ref="I28:I31"/>
     <mergeCell ref="J28:J31"/>
     <mergeCell ref="B33:B39"/>
@@ -2473,6 +2520,44 @@
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="E28:E31"/>
     <mergeCell ref="F28:F31"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:I14"/>
+    <mergeCell ref="J11:J14"/>
+    <mergeCell ref="B15:J19"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B3:J6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="J7:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2526,89 +2611,89 @@
       <c r="A3" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2616,8 +2701,8 @@
       <c r="A8" s="5">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -2630,8 +2715,8 @@
       <c r="A9" s="5">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -2644,8 +2729,8 @@
       <c r="A10" s="5">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -2658,31 +2743,31 @@
       <c r="A11" s="5">
         <v>0.5</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2690,8 +2775,8 @@
       <c r="A12" s="5">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -2704,8 +2789,8 @@
       <c r="A13" s="5">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -2718,8 +2803,8 @@
       <c r="A14" s="5">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -2732,103 +2817,103 @@
       <c r="A15" s="5">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2836,8 +2921,8 @@
       <c r="A21" s="5">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -2850,8 +2935,8 @@
       <c r="A22" s="5">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
@@ -2864,8 +2949,8 @@
       <c r="A23" s="5">
         <v>0.625</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -2878,27 +2963,27 @@
       <c r="A24" s="5">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -2907,7 +2992,7 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="14"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -2921,7 +3006,7 @@
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -2935,7 +3020,7 @@
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
@@ -2946,34 +3031,34 @@
       <c r="A28" s="5">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="14"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="14"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -2984,10 +3069,10 @@
       <c r="A30" s="5">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="14"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="14"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
@@ -2998,10 +3083,10 @@
       <c r="A31" s="5">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
@@ -3026,13 +3111,13 @@
       <c r="A33" s="5">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E33" s="4"/>
@@ -3046,8 +3131,8 @@
       <c r="A34" s="5">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="11"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -3060,8 +3145,8 @@
       <c r="A35" s="5">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="11"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -3074,8 +3159,8 @@
       <c r="A36" s="5">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="11"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -3088,8 +3173,8 @@
       <c r="A37" s="5">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="11"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -3102,8 +3187,8 @@
       <c r="A38" s="5">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="11"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -3116,8 +3201,8 @@
       <c r="A39" s="5">
         <v>0.79166666666666197</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
       <c r="D39" s="12"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -3133,44 +3218,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="B3:J6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="J7:J10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="J11:J14"/>
-    <mergeCell ref="B15:J19"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
     <mergeCell ref="I28:I31"/>
     <mergeCell ref="J28:J31"/>
     <mergeCell ref="B33:B39"/>
@@ -3183,6 +3230,44 @@
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="E28:E31"/>
     <mergeCell ref="F28:F31"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:I14"/>
+    <mergeCell ref="J11:J14"/>
+    <mergeCell ref="B15:J19"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B3:J6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="J7:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3291,13 +3376,13 @@
       <c r="A7" s="5">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="35" t="s">
@@ -3365,31 +3450,31 @@
       <c r="A11" s="5">
         <v>0.5</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3439,103 +3524,103 @@
       <c r="A15" s="5">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3585,27 +3670,27 @@
       <c r="A24" s="5">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -3614,7 +3699,7 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="14"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -3628,7 +3713,7 @@
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -3642,7 +3727,7 @@
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
@@ -3653,34 +3738,34 @@
       <c r="A28" s="5">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="14"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="14"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
@@ -3691,10 +3776,10 @@
       <c r="A30" s="5">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="14"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="14"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
@@ -3705,10 +3790,10 @@
       <c r="A31" s="5">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
@@ -3733,13 +3818,13 @@
       <c r="A33" s="5">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E33" s="2"/>
@@ -3753,8 +3838,8 @@
       <c r="A34" s="5">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="11"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -3767,8 +3852,8 @@
       <c r="A35" s="5">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="11"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -3781,8 +3866,8 @@
       <c r="A36" s="5">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="11"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -3795,8 +3880,8 @@
       <c r="A37" s="5">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="11"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -3809,8 +3894,8 @@
       <c r="A38" s="5">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="11"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -3823,8 +3908,8 @@
       <c r="A39" s="5">
         <v>0.79166666666666197</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
       <c r="D39" s="12"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -3840,44 +3925,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="B3:J6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="J7:J10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="I11:I14"/>
-    <mergeCell ref="J11:J14"/>
-    <mergeCell ref="B15:J19"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
     <mergeCell ref="I28:I31"/>
     <mergeCell ref="J28:J31"/>
     <mergeCell ref="B33:B39"/>
@@ -3890,6 +3937,44 @@
     <mergeCell ref="D28:D31"/>
     <mergeCell ref="E28:E31"/>
     <mergeCell ref="F28:F31"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="H11:H14"/>
+    <mergeCell ref="I11:I14"/>
+    <mergeCell ref="J11:J14"/>
+    <mergeCell ref="B15:J19"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B3:J6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="J7:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3897,10 +3982,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE242408-A213-49C5-A8C5-09FACDF545F8}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3908,10 +3993,11 @@
     <col min="2" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15.5703125" customWidth="1"/>
-    <col min="7" max="7" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="57" customWidth="1"/>
+    <col min="8" max="8" width="81.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -3928,7 +4014,7 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -3936,376 +4022,409 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="66"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="45" t="s">
+      <c r="B7" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="72"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="61"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="39"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="73"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="57" t="s">
+      <c r="B9" s="39"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="40" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="68" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="39"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="69"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>0.5</v>
       </c>
-      <c r="B11" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="45" t="s">
+      <c r="B11" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="47"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="54"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="72"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="61"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="39"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="73"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="57" t="s">
+      <c r="B13" s="39"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="57" t="s">
+      <c r="G13" s="40" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="68" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="69"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="77"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="75"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="77"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="75"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="77"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="75"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="77"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="78"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="80"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="46"/>
-      <c r="G20" s="47"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="68"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="39"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="74"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="50"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="39"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="81"/>
+      <c r="H22" s="74"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>0.625</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="51"/>
       <c r="F23" s="52"/>
-      <c r="G23" s="53"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="52"/>
+      <c r="H23" s="69"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="82" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="70"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>0.64583333333333304</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="14"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="83"/>
+      <c r="H25" s="85"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>0.65625</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
-      <c r="E26" s="14"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="83"/>
+      <c r="H26" s="85"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>0.66666666666666696</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="84"/>
+      <c r="H27" s="71"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="86"/>
+      <c r="H28" s="68"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="14"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="83"/>
+      <c r="H29" s="74"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="14"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="83"/>
+      <c r="H30" s="74"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>0.70833333333333304</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="15"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="84"/>
+      <c r="H31" s="69"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>0.718749999999999</v>
       </c>
@@ -4320,13 +4439,13 @@
       <c r="A33" s="5">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="26" t="s">
+      <c r="B33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E33" s="4"/>
@@ -4405,21 +4524,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="B7:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="E7:G8"/>
-    <mergeCell ref="B15:G19"/>
-    <mergeCell ref="B20:D23"/>
-    <mergeCell ref="E20:G23"/>
-    <mergeCell ref="B11:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E11:G12"/>
+  <mergeCells count="33">
+    <mergeCell ref="B15:H19"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="B3:H6"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="E7:H8"/>
+    <mergeCell ref="E11:H12"/>
     <mergeCell ref="B33:B39"/>
     <mergeCell ref="C33:C39"/>
     <mergeCell ref="D33:D39"/>
@@ -4435,6 +4548,16 @@
     <mergeCell ref="D24:D27"/>
     <mergeCell ref="E24:E27"/>
     <mergeCell ref="F24:F27"/>
+    <mergeCell ref="B20:D23"/>
+    <mergeCell ref="E20:G23"/>
+    <mergeCell ref="B11:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="B7:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4472,7 +4595,7 @@
       <c r="A3" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="57" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4480,25 +4603,25 @@
       <c r="A4" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="62"/>
+      <c r="B4" s="57"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="62"/>
+      <c r="B5" s="57"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="62"/>
+      <c r="B6" s="57"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="60" t="s">
         <v>34</v>
       </c>
     </row>
@@ -4506,49 +4629,49 @@
       <c r="A8" s="5">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="65"/>
+      <c r="B8" s="60"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="65"/>
+      <c r="B9" s="60"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="65"/>
+      <c r="B10" s="60"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>0.5</v>
       </c>
-      <c r="B11" s="65"/>
+      <c r="B11" s="60"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="65"/>
+      <c r="B12" s="60"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="65"/>
+      <c r="B13" s="60"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="65"/>
+      <c r="B14" s="60"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="61" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4556,25 +4679,25 @@
       <c r="A16" s="5">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="67"/>
+      <c r="B16" s="62"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="67"/>
+      <c r="B17" s="62"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="67"/>
+      <c r="B18" s="62"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="68"/>
+      <c r="B19" s="63"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -4588,7 +4711,7 @@
       <c r="A21" s="5">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="60" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4596,37 +4719,37 @@
       <c r="A22" s="5">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="65"/>
+      <c r="B22" s="60"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>0.625</v>
       </c>
-      <c r="B23" s="65"/>
+      <c r="B23" s="60"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="65"/>
+      <c r="B24" s="60"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="65"/>
+      <c r="B25" s="60"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="65"/>
+      <c r="B26" s="60"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="65" t="s">
+      <c r="B27" s="60" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4634,19 +4757,19 @@
       <c r="A28" s="5">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="65"/>
+      <c r="B28" s="60"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="65"/>
+      <c r="B29" s="60"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="64" t="s">
+      <c r="B30" s="59" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4654,19 +4777,19 @@
       <c r="A31" s="5">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B31" s="64"/>
+      <c r="B31" s="59"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="64"/>
+      <c r="B32" s="59"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="57" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4674,25 +4797,25 @@
       <c r="A34" s="5">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="62"/>
+      <c r="B34" s="57"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="62"/>
+      <c r="B35" s="57"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="62"/>
+      <c r="B36" s="57"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="63" t="s">
+      <c r="B37" s="58" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4700,31 +4823,31 @@
       <c r="A38" s="5">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="63"/>
+      <c r="B38" s="58"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>0.79166666666666197</v>
       </c>
-      <c r="B39" s="63"/>
+      <c r="B39" s="58"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>0.80208333333332804</v>
       </c>
-      <c r="B40" s="63"/>
+      <c r="B40" s="58"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>0.812499999999994</v>
       </c>
-      <c r="B41" s="63"/>
+      <c r="B41" s="58"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>0.82291666666665997</v>
       </c>
-      <c r="B42" s="62" t="s">
+      <c r="B42" s="57" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4732,19 +4855,19 @@
       <c r="A43" s="5">
         <v>0.83333333333332604</v>
       </c>
-      <c r="B43" s="62"/>
+      <c r="B43" s="57"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>0.84374999999999201</v>
       </c>
-      <c r="B44" s="62"/>
+      <c r="B44" s="57"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>0.85416666666665797</v>
       </c>
-      <c r="B45" s="64" t="s">
+      <c r="B45" s="59" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4752,37 +4875,37 @@
       <c r="A46" s="5">
         <v>0.86458333333332404</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="59"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>0.87499999999999101</v>
       </c>
-      <c r="B47" s="64"/>
+      <c r="B47" s="59"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>0.88541666666665697</v>
       </c>
-      <c r="B48" s="64"/>
+      <c r="B48" s="59"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>0.89583333333332305</v>
       </c>
-      <c r="B49" s="64"/>
+      <c r="B49" s="59"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>0.90624999999998901</v>
       </c>
-      <c r="B50" s="64"/>
+      <c r="B50" s="59"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>0.91666666666665497</v>
       </c>
-      <c r="B51" s="64"/>
+      <c r="B51" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Enhance student timetable generation by adding a new "Harp Regulation Workshop" activity and refining logic for handling lessons with pianists. Introduce debug output for student C5 to assist in troubleshooting. Update room mappings in CSV files for improved accuracy.
</commit_message>
<xml_diff>
--- a/input/harp-campA-time-table.xlsx
+++ b/input/harp-campA-time-table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapmi\Desktop\summer-camp-time-table\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB98613-15C6-404E-A01C-E3365E406C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4A228C-F75D-49B0-9150-9899047401A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1508" windowWidth="18975" windowHeight="11272" activeTab="5" xr2:uid="{E318233D-D99F-47E3-BC58-6A555949ADA4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{E318233D-D99F-47E3-BC58-6A555949ADA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="49">
   <si>
     <t>Sivan MEGAN</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Break</t>
   </si>
   <si>
-    <t>Group 2, 5, 8, 9 Acting Class (Room Acting Class)</t>
-  </si>
-  <si>
     <t>Group 6
 (Room Ivy)</t>
   </si>
@@ -109,9 +106,6 @@
     <t>Group 8</t>
   </si>
   <si>
-    <t>Group 1, 3, 4, 6, 7 Acting Class (Room Acting Class)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Faculty Rehearsal </t>
   </si>
   <si>
@@ -139,14 +133,6 @@
   <si>
     <t>Briefing for Saturday
 (Room zzz)</t>
-  </si>
-  <si>
-    <t>Group 2, 5, 8, 9 Group Activity
-(Room Group Activity)</t>
-  </si>
-  <si>
-    <t>Group 1, 3, 4, 6, 7 Group Activity
-(Room Group Activity)</t>
   </si>
   <si>
     <t>Check in Maritime Museum
@@ -202,16 +188,22 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Harp MasterClass by Liya HUANG**
-H1, H7. H8</t>
-  </si>
-  <si>
     <t>Harp MasterClass by Sivan MEGAN**
 H2, H4, H9</t>
   </si>
   <si>
     <t>Harp MasterClass by Gwyneth WENTINK**
 H3, H5, H6</t>
+  </si>
+  <si>
+    <t>Group 2, 5, 7, 9 Acting Class (Room Acting Class)</t>
+  </si>
+  <si>
+    <t>Group 1, 3, 4, 6, 8 Acting Class (Room Acting Class)</t>
+  </si>
+  <si>
+    <t>Harp MasterClass by Liya HUANG**
+H1, H7, H8</t>
   </si>
 </sst>
 </file>
@@ -440,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -533,32 +525,26 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -907,7 +893,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="E24" sqref="E24:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -917,7 +903,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -937,7 +923,7 @@
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1309,19 +1295,19 @@
         <v>14</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="25" t="s">
         <v>17</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>18</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -1377,16 +1363,16 @@
         <v>16</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -1454,13 +1440,13 @@
         <v>0.72916666666666496</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -1626,7 +1612,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="E24" sqref="E24:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -1636,7 +1622,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1656,7 +1642,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1673,7 +1659,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -1733,7 +1719,9 @@
       <c r="B7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="24"/>
+      <c r="C7" s="24" t="s">
+        <v>16</v>
+      </c>
       <c r="D7" s="24" t="s">
         <v>8</v>
       </c>
@@ -2014,7 +2002,7 @@
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>0.63541666666666696</v>
       </c>
@@ -2022,19 +2010,19 @@
         <v>14</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="25" t="s">
         <v>17</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>18</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -2082,7 +2070,7 @@
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
         <v>0.67708333333333304</v>
       </c>
@@ -2090,16 +2078,16 @@
         <v>16</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -2167,13 +2155,13 @@
         <v>0.72916666666666496</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2333,7 +2321,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="E24" sqref="E24:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -2343,7 +2331,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -2363,7 +2351,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2380,7 +2368,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -2456,7 +2444,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>9</v>
@@ -2530,7 +2518,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>9</v>
@@ -2727,7 +2715,7 @@
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>0.63541666666666696</v>
       </c>
@@ -2735,19 +2723,19 @@
         <v>14</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="25" t="s">
         <v>17</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>18</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -2795,7 +2783,7 @@
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
         <v>0.67708333333333304</v>
       </c>
@@ -2803,16 +2791,16 @@
         <v>16</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -2880,13 +2868,13 @@
         <v>0.72916666666666496</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -3046,7 +3034,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView zoomScale="103" workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="E24" sqref="E24:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -3056,7 +3044,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -3076,7 +3064,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -3086,7 +3074,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -3441,19 +3429,19 @@
         <v>14</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="25" t="s">
         <v>17</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="25" t="s">
-        <v>18</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
@@ -3509,16 +3497,16 @@
         <v>16</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F28" s="25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -3586,13 +3574,13 @@
         <v>0.72916666666666496</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -3751,8 +3739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE242408-A213-49C5-A8C5-09FACDF545F8}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -3764,7 +3752,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -3781,7 +3769,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -3792,7 +3780,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="34"/>
@@ -3841,27 +3829,27 @@
       <c r="A7" s="5">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="38" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
       <c r="H7" s="38" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
@@ -3871,9 +3859,9 @@
       <c r="A9" s="5">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
       <c r="E9" s="38" t="s">
         <v>7</v>
       </c>
@@ -3889,39 +3877,39 @@
       <c r="A10" s="5">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>0.5</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="B11" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
       <c r="E11" s="38" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
       <c r="H11" s="38" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
       <c r="E12" s="38"/>
       <c r="F12" s="38"/>
       <c r="G12" s="38"/>
@@ -3931,9 +3919,9 @@
       <c r="A13" s="5">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
       <c r="E13" s="38" t="s">
         <v>10</v>
       </c>
@@ -3949,85 +3937,85 @@
       <c r="A14" s="5">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="38"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
+      <c r="B20" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
       <c r="G20" s="38"/>
@@ -4037,59 +4025,59 @@
       <c r="A21" s="5">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>0.625</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="42" t="s">
+      <c r="C24" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="40" t="s">
-        <v>18</v>
+      <c r="E24" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="36" t="s">
+        <v>17</v>
       </c>
       <c r="H24" s="38"/>
     </row>
@@ -4097,56 +4085,56 @@
       <c r="A25" s="5">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="5">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="5">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F28" s="40" t="s">
-        <v>25</v>
+      <c r="C28" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>23</v>
       </c>
       <c r="G28" s="38"/>
       <c r="H28" s="38"/>
@@ -4155,37 +4143,37 @@
       <c r="A29" s="5">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="5">
@@ -4203,13 +4191,13 @@
         <v>0.72916666666666496</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -4295,6 +4283,11 @@
     <mergeCell ref="D24:D27"/>
     <mergeCell ref="E24:E27"/>
     <mergeCell ref="F24:F27"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="B20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="G20:G23"/>
     <mergeCell ref="B3:H6"/>
     <mergeCell ref="B15:H19"/>
     <mergeCell ref="B7:D10"/>
@@ -4307,11 +4300,6 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="E11:G12"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="B20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="G20:G23"/>
     <mergeCell ref="B33:B39"/>
     <mergeCell ref="C33:C39"/>
     <mergeCell ref="D33:D39"/>
@@ -4333,7 +4321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46B8B14-C1FC-4368-9C36-E38F728D68D9}">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -4344,41 +4332,41 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B2" s="45" t="s">
-        <v>32</v>
+      <c r="B2" s="42" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="42"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>0.4375</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="42"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B5" s="45"/>
+      <c r="B5" s="42"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>0.45833333333333298</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -4427,40 +4415,40 @@
       <c r="A14" s="5">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B14" s="46" t="s">
-        <v>34</v>
+      <c r="B14" s="44" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B15" s="47"/>
+      <c r="B15" s="45"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>0.5625</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="45"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B17" s="47"/>
+      <c r="B17" s="45"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B18" s="48"/>
+      <c r="B18" s="46"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>0.59375</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
@@ -4468,7 +4456,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B20" s="43" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
@@ -4506,7 +4494,7 @@
         <v>0.66666666666666696</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
@@ -4525,27 +4513,27 @@
       <c r="A29" s="5">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B29" s="40" t="s">
-        <v>38</v>
+      <c r="B29" s="36" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B30" s="40"/>
+      <c r="B30" s="36"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
         <v>0.718749999999999</v>
       </c>
-      <c r="B31" s="40"/>
+      <c r="B31" s="36"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="5">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B32" s="45" t="s">
+      <c r="B32" s="42" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4553,115 +4541,115 @@
       <c r="A33" s="5">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B33" s="45"/>
+      <c r="B33" s="42"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="5">
         <v>0.749999999999997</v>
       </c>
-      <c r="B34" s="45"/>
+      <c r="B34" s="42"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B35" s="45"/>
+      <c r="B35" s="42"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="5">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B36" s="36" t="s">
-        <v>39</v>
+      <c r="B36" s="40" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="5">
         <v>0.781249999999996</v>
       </c>
-      <c r="B37" s="36"/>
+      <c r="B37" s="40"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="5">
         <v>0.79166666666666197</v>
       </c>
-      <c r="B38" s="36"/>
+      <c r="B38" s="40"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="5">
         <v>0.80208333333332804</v>
       </c>
-      <c r="B39" s="36"/>
+      <c r="B39" s="40"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="5">
         <v>0.812499999999994</v>
       </c>
-      <c r="B40" s="36"/>
+      <c r="B40" s="40"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="5">
         <v>0.82291666666665997</v>
       </c>
-      <c r="B41" s="45" t="s">
-        <v>40</v>
+      <c r="B41" s="42" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="5">
         <v>0.83333333333332604</v>
       </c>
-      <c r="B42" s="45"/>
+      <c r="B42" s="42"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="5">
         <v>0.84374999999999201</v>
       </c>
-      <c r="B43" s="45"/>
+      <c r="B43" s="42"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="5">
         <v>0.85416666666665797</v>
       </c>
-      <c r="B44" s="40" t="s">
-        <v>41</v>
+      <c r="B44" s="36" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="5">
         <v>0.86458333333332404</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="36"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" s="5">
         <v>0.87499999999999101</v>
       </c>
-      <c r="B46" s="40"/>
+      <c r="B46" s="36"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="5">
         <v>0.88541666666665697</v>
       </c>
-      <c r="B47" s="40"/>
+      <c r="B47" s="36"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="5">
         <v>0.89583333333332305</v>
       </c>
-      <c r="B48" s="40"/>
+      <c r="B48" s="36"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" s="5">
         <v>0.90624999999998901</v>
       </c>
-      <c r="B49" s="40"/>
+      <c r="B49" s="36"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" s="5">
         <v>0.91666666666665497</v>
       </c>
-      <c r="B50" s="40"/>
+      <c r="B50" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>